<commit_message>
Remove outdated Excel files and add script to calculate last month's date range
</commit_message>
<xml_diff>
--- a/output/2025/03/26/data_FEB2025.xlsx
+++ b/output/2025/03/26/data_FEB2025.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2045,6 +2045,378 @@
         </is>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>AA202400050262247</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>050</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>ANWA ODUMO</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>98765422789</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>ANWA ODUMO</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Canada</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Personal Travel Allowance (PTA)</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>REPAYMENT OF FOREIGN LOANS</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>2025-02-23</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>100.0</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>AA202400050262134</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>050</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>ANWA ODUMO</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>98765422789</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>A and T Medical services</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>United States of America</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Maintenance/Upkeep</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>REPAYMENT OF FOREIGN LOANS</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>2025-02-21</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>AA202400050262413</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>050</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>ANWA ODUMO</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>98765422789</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>A and T Medical services</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>United States of America</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>CONSULTANCY FEES</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>REPAYMENT OF FOREIGN LOANS</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>2025-02-09</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>100.0</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>AA202400050262247</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>050</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>ANWA ODUMO</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>98765422789</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>ANWA ODUMO</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Canada</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Personal Travel Allowance (PTA)</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>REPAYMENT OF FOREIGN LOANS</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>2025-02-23</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>100.0</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>AA202400050262134</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>050</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>ANWA ODUMO</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>98765422789</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>A and T Medical services</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>United States of America</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Maintenance/Upkeep</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>REPAYMENT OF FOREIGN LOANS</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>2025-02-21</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>AA202400050262413</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>050</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>ANWA ODUMO</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>98765422789</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>A and T Medical services</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>United States of America</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>CONSULTANCY FEES</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>REPAYMENT OF FOREIGN LOANS</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>2025-02-09</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>100.0</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>